<commit_message>
Generalize Excel and CSV CourseWriters and improve template loading
</commit_message>
<xml_diff>
--- a/src/spz/spz/templates/export/course.xlsx
+++ b/src/spz/spz/templates/export/course.xlsx
@@ -5,19 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tims\Code\Workspace\SPZ\other\export_test\xlsx_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\spz-signup\src\spz\spz\templates\export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2657052-DBAE-4390-B2C0-43103A7F8292}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFF31EE-887B-489A-8BC0-F5475133A76F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{4B71185F-4713-4773-B9E1-358926F1CBA9}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="16608" windowHeight="10536" xr2:uid="{4B71185F-4713-4773-B9E1-358926F1CBA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Kursliste" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="FILL_IN" comment="course.full_name;applicant.last_name;applicant.first_name;applicant.origin.short_name;applicant.tag;applicant.mail;applicant.phone">Kursliste!$A$2:$G$99</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Kurs</t>
   </si>
@@ -57,6 +54,27 @@
   </si>
   <si>
     <t>Telefon</t>
+  </si>
+  <si>
+    <t>course.full_name</t>
+  </si>
+  <si>
+    <t>applicant.last_name</t>
+  </si>
+  <si>
+    <t>applicant.first_name</t>
+  </si>
+  <si>
+    <t>applicant.origin.short_name</t>
+  </si>
+  <si>
+    <t>applicant.tag</t>
+  </si>
+  <si>
+    <t>applicant.mail</t>
+  </si>
+  <si>
+    <t>applicant.phone</t>
   </si>
 </sst>
 </file>
@@ -107,9 +125,7 @@
         <color theme="4" tint="0.39997558519241921"/>
       </left>
       <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </bottom>
@@ -118,9 +134,7 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </bottom>
@@ -131,9 +145,7 @@
       <right style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </bottom>
@@ -152,7 +164,46 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -163,6 +214,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5D09895E-C005-41D3-9442-936E62EB3CB4}" name="DATA" displayName="DATA" ref="A1:G2" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:G2" xr:uid="{B53292A9-20AD-45CE-8CEF-0A3DC228558B}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{09C0ACB9-37EC-449F-86F8-6FCCF25208F9}" name="Kurs"/>
+    <tableColumn id="2" xr3:uid="{D53728A0-E265-4FD0-BCF9-400D7E340283}" name="Nachname"/>
+    <tableColumn id="3" xr3:uid="{61CDCC7B-455E-4071-9C6D-B5486327D145}" name="Vorname"/>
+    <tableColumn id="4" xr3:uid="{4082E060-7384-4FA6-A2A9-067B9C4C4371}" name="Hochschule"/>
+    <tableColumn id="5" xr3:uid="{F393C0C9-D396-4C77-AB90-995CBB680942}" name="Matrikelnummer"/>
+    <tableColumn id="6" xr3:uid="{209CC84C-AE63-4F0D-B0A3-0735F3C4B25B}" name="E-Mail"/>
+    <tableColumn id="7" xr3:uid="{39700E58-70E4-4833-9860-BA3DD0BA5858}" name="Telefon"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -462,15 +529,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A45634-26AD-4053-BD2F-210A0537753F}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G99"/>
+      <selection activeCell="E1" sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="11.15625" customWidth="1"/>
+    <col min="4" max="4" width="11.7890625" customWidth="1"/>
+    <col min="5" max="5" width="16.3671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,9 +563,35 @@
       </c>
       <c r="G1" s="3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add zip-excel export writer
</commit_message>
<xml_diff>
--- a/src/spz/spz/templates/export/course.xlsx
+++ b/src/spz/spz/templates/export/course.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\spz-signup\src\spz\spz\templates\export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFF31EE-887B-489A-8BC0-F5475133A76F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE6AAAA-12F9-436C-8B62-9FE84DF33BFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="16608" windowHeight="10536" xr2:uid="{4B71185F-4713-4773-B9E1-358926F1CBA9}"/>
   </bookViews>
@@ -65,9 +65,6 @@
     <t>applicant.first_name</t>
   </si>
   <si>
-    <t>applicant.origin.short_name</t>
-  </si>
-  <si>
     <t>applicant.tag</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>applicant.phone</t>
+  </si>
+  <si>
+    <t>applicant.origin.name</t>
   </si>
 </sst>
 </file>
@@ -166,6 +166,20 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -189,20 +203,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -217,7 +217,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5D09895E-C005-41D3-9442-936E62EB3CB4}" name="DATA" displayName="DATA" ref="A1:G2" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5D09895E-C005-41D3-9442-936E62EB3CB4}" name="DATA" displayName="DATA" ref="A1:G2" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:G2" xr:uid="{B53292A9-20AD-45CE-8CEF-0A3DC228558B}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{09C0ACB9-37EC-449F-86F8-6FCCF25208F9}" name="Kurs"/>
@@ -532,7 +532,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="A1:G2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -576,16 +576,16 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>